<commit_message>
changed the caliberation from 2 sec to 5 sec
</commit_message>
<xml_diff>
--- a/seconds_calculator.xlsx
+++ b/seconds_calculator.xlsx
@@ -363,7 +363,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -375,8 +375,8 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
-        <v>1.5018674201649999E+18</v>
+      <c r="B1">
+        <v>1.501867429108E+18</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -384,7 +384,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1.5018674215820001E+18</v>
+        <v>1.50186743374E+18</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -393,16 +393,16 @@
       </c>
       <c r="B3" s="1">
         <f>B2-B1</f>
-        <v>1417000192</v>
+        <v>4632000000</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <f>B3/POWER(10,9)</f>
-        <v>1.4170001919999999</v>
+        <v>4.6319999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
beginning works on the model development basics
</commit_message>
<xml_diff>
--- a/seconds_calculator.xlsx
+++ b/seconds_calculator.xlsx
@@ -363,7 +363,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -376,7 +376,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>1.501867429108E+18</v>
+        <v>1.5018674201649999E+18</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -384,7 +384,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1.50186743374E+18</v>
+        <v>1.5018674291219999E+18</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -393,7 +393,7 @@
       </c>
       <c r="B3" s="1">
         <f>B2-B1</f>
-        <v>4632000000</v>
+        <v>8956999936</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -402,7 +402,7 @@
       </c>
       <c r="B4">
         <f>B3/POWER(10,9)</f>
-        <v>4.6319999999999997</v>
+        <v>8.9569999360000008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
analysis on training file sets
</commit_message>
<xml_diff>
--- a/seconds_calculator.xlsx
+++ b/seconds_calculator.xlsx
@@ -11,7 +11,29 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$B$2</definedName>
+    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$B$2</definedName>
+    <definedName name="solver_lin" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$B$4</definedName>
+    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_rel1" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">Sheet1!$B$1</definedName>
+    <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_tim" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_tol" localSheetId="0" hidden="1">0.05</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">15</definedName>
+  </definedNames>
+  <calcPr calcId="124519" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -34,7 +56,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -42,16 +64,317 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -59,16 +382,207 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -363,7 +877,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -375,7 +889,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="2">
         <v>1.5018674201649999E+18</v>
       </c>
     </row>
@@ -383,17 +897,17 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1.5018674291219999E+18</v>
+      <c r="B2" s="3">
+        <v>1.5018675053260001E+18</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <f>B2-B1</f>
-        <v>8956999936</v>
+        <v>85161000192</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -402,7 +916,7 @@
       </c>
       <c r="B4">
         <f>B3/POWER(10,9)</f>
-        <v>8.9569999360000008</v>
+        <v>85.161000192000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
December 5th CaseA all file analysis completed
</commit_message>
<xml_diff>
--- a/seconds_calculator.xlsx
+++ b/seconds_calculator.xlsx
@@ -877,7 +877,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -889,8 +889,8 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2">
-        <v>1.5018674201649999E+18</v>
+      <c r="B1" s="3">
+        <v>1.510873871772E+18</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -898,7 +898,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <v>1.5018675053260001E+18</v>
+        <v>1.5108740236209999E+18</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -907,7 +907,7 @@
       </c>
       <c r="B3" s="2">
         <f>B2-B1</f>
-        <v>85161000192</v>
+        <v>151848999936</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -916,7 +916,7 @@
       </c>
       <c r="B4">
         <f>B3/POWER(10,9)</f>
-        <v>85.161000192000003</v>
+        <v>151.84899993600001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
running model on test files part 5 to 8; December 5th
</commit_message>
<xml_diff>
--- a/seconds_calculator.xlsx
+++ b/seconds_calculator.xlsx
@@ -877,7 +877,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -890,7 +890,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3">
-        <v>1.510873871772E+18</v>
+        <v>1.510872012008E+18</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -898,7 +898,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <v>1.5108740236209999E+18</v>
+        <v>1.5108722218739999E+18</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -907,7 +907,7 @@
       </c>
       <c r="B3" s="2">
         <f>B2-B1</f>
-        <v>151848999936</v>
+        <v>209865999872</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -916,7 +916,7 @@
       </c>
       <c r="B4">
         <f>B3/POWER(10,9)</f>
-        <v>151.84899993600001</v>
+        <v>209.865999872</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Documentation included to the repo
</commit_message>
<xml_diff>
--- a/seconds_calculator.xlsx
+++ b/seconds_calculator.xlsx
@@ -33,7 +33,7 @@
     <definedName name="solver_typ" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">15</definedName>
   </definedNames>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -890,7 +890,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3">
-        <v>1.510872012008E+18</v>
+        <v>1.5018677321969999E+18</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -898,7 +898,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <v>1.5108722218739999E+18</v>
+        <v>1.5018679661849999E+18</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -907,7 +907,7 @@
       </c>
       <c r="B3" s="2">
         <f>B2-B1</f>
-        <v>209865999872</v>
+        <v>233988000000</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -916,7 +916,7 @@
       </c>
       <c r="B4">
         <f>B3/POWER(10,9)</f>
-        <v>209.865999872</v>
+        <v>233.988</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uploading analysis on Case E - additional file given
</commit_message>
<xml_diff>
--- a/seconds_calculator.xlsx
+++ b/seconds_calculator.xlsx
@@ -890,7 +890,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3">
-        <v>1.5018677321969999E+18</v>
+        <v>1.5108736928179999E+18</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -898,7 +898,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <v>1.5018679661849999E+18</v>
+        <v>1.510873839248E+18</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -907,7 +907,7 @@
       </c>
       <c r="B3" s="2">
         <f>B2-B1</f>
-        <v>233988000000</v>
+        <v>146430000128</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -916,7 +916,7 @@
       </c>
       <c r="B4">
         <f>B3/POWER(10,9)</f>
-        <v>233.988</v>
+        <v>146.43000012799999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>